<commit_message>
[06-18-2018]-Updated Data in Both the Files.
</commit_message>
<xml_diff>
--- a/src/main/java/Data/Data.xlsx
+++ b/src/main/java/Data/Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Shows</t>
   </si>
@@ -38,15 +38,11 @@
   <si>
     <t>American Grit</t>
   </si>
-  <si>
-    <t>duplicate</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -455,12 +451,12 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.83203125" collapsed="true"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -475,17 +471,13 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
@@ -497,9 +489,7 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2"/>

</xml_diff>